<commit_message>
Inizio della progettazione dell'App
</commit_message>
<xml_diff>
--- a/shareApp.xlsx
+++ b/shareApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ciro\Documents\GitHub\ShareApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FCB70E-4B93-4C35-A0BB-EFF5D68A9061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4BDD66-B24A-4C2B-8412-4DF38C4EC0AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3578F0B-86F4-46CC-A856-AE6BB5A4169E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>Azione desiderata</t>
   </si>
@@ -162,19 +162,6 @@
   <si>
     <t>{
     "status": "success",
-    "authKey": "76U...kzb",
-    "avatar": "generic.png"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "request": "getAvatar",
-    "authentication": "IEG...Dd2"
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "success",
     "avatar": "generic.png"
 }</t>
   </si>
@@ -235,10 +222,6 @@
   <si>
     <t>Rimuovi utente
 dai contatti</t>
-  </si>
-  <si>
-    <t>Ottieni avatar
-corrente</t>
   </si>
   <si>
     <t>Il Sender fa richiesta
@@ -316,6 +299,29 @@
     "authentication": "76U...kzb",
     "myPhoneNumber": "333...761",
     "contacts": ["339…485", "388…956"]
+}</t>
+  </si>
+  <si>
+    <t>Ottieni user corrente</t>
+  </si>
+  <si>
+    <t>{
+    "request": "getCurrentUser",
+    "authentication": "IEG...Dd2"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "authKey": "76U...kzb"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "user_ID": 4,
+    "username": "pippo",
+    "avatar": "generic.png"
 }</t>
   </si>
 </sst>
@@ -734,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D127C033-A9B8-4410-B122-7AA03B47CAAB}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,7 +757,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -762,7 +768,7 @@
     </row>
     <row r="2" spans="1:7" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -788,10 +794,10 @@
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
@@ -802,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
@@ -811,71 +817,77 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -883,10 +895,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -902,52 +914,52 @@
     </row>
     <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -955,10 +967,10 @@
     </row>
     <row r="16" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -966,7 +978,7 @@
     </row>
     <row r="18" spans="1:7" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -977,7 +989,7 @@
     </row>
     <row r="19" spans="1:7" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>

</xml_diff>

<commit_message>
Avanzamenti nello sviluppo dell'App
</commit_message>
<xml_diff>
--- a/shareApp.xlsx
+++ b/shareApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ciro\Documents\GitHub\ShareApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4BDD66-B24A-4C2B-8412-4DF38C4EC0AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47D0ED8-2687-428D-B864-1FD0EA37FA3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3578F0B-86F4-46CC-A856-AE6BB5A4169E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Azione desiderata</t>
   </si>
@@ -323,6 +323,16 @@
     "username": "pippo",
     "avatar": "generic.png"
 }</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": "USER_NOT_FOUND"
+}</t>
+  </si>
+  <si>
+    <t>L'utente indicato non è
+stato trovato</t>
   </si>
 </sst>
 </file>
@@ -740,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D127C033-A9B8-4410-B122-7AA03B47CAAB}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,6 +888,12 @@
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">

</xml_diff>

<commit_message>
Sender upload parzialmente implementato
</commit_message>
<xml_diff>
--- a/shareApp.xlsx
+++ b/shareApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ciro\Documents\GitHub\ShareApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47D0ED8-2687-428D-B864-1FD0EA37FA3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EDD929-3DF7-4A8E-846E-84AE511F3B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3578F0B-86F4-46CC-A856-AE6BB5A4169E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Azione desiderata</t>
   </si>
@@ -334,12 +334,28 @@
     <t>L'utente indicato non è
 stato trovato</t>
   </si>
+  <si>
+    <t>Risposta (errore 3)</t>
+  </si>
+  <si>
+    <t>Possibili cause (errore 3)</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": "USERS_NOT_CONNECTED"
+}</t>
+  </si>
+  <si>
+    <t>Il ricevente non ha l'utente
+corrente nella rubrica</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +373,12 @@
     <font>
       <sz val="36"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -436,9 +458,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D64A82E-31C2-4D9B-9154-C73794CDC280}" name="Tabella2" displayName="Tabella2" ref="A4:G16" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A4:G16" xr:uid="{AAF4FC5C-BCC3-4737-80E5-78CE43E9DF93}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D64A82E-31C2-4D9B-9154-C73794CDC280}" name="Tabella2" displayName="Tabella2" ref="A4:I16" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A4:I16" xr:uid="{AAF4FC5C-BCC3-4737-80E5-78CE43E9DF93}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{9FF0D9C1-46F2-4E1C-AB10-44965E917E07}" name="Azione desiderata" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{3BA924DE-7D49-423F-9A32-CCA64D9F8D7C}" name="Esempio di input valido" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{7AEFBF60-F909-4255-A240-E9B3F50C5813}" name="Risposta (successo)" dataDxfId="2"/>
@@ -446,6 +468,8 @@
     <tableColumn id="5" xr3:uid="{4015E837-6B88-4EFE-ACF5-A05484234112}" name="Possibili cause (errore 1)" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{B194EE7C-D861-4EBC-80D9-D9ADB094934A}" name="Risposta (errore 2)"/>
     <tableColumn id="7" xr3:uid="{5B99A82B-8404-4D92-81C7-A8FDD2194DF3}" name="Possibili cause (errore 2)"/>
+    <tableColumn id="8" xr3:uid="{32F33ECD-944D-420A-9826-12534A9C8574}" name="Risposta (errore 3)"/>
+    <tableColumn id="9" xr3:uid="{45250021-96FF-4264-B222-76A9E6F72C46}" name="Possibili cause (errore 3)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -748,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D127C033-A9B8-4410-B122-7AA03B47CAAB}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,9 +787,11 @@
     <col min="5" max="5" width="23.88671875" style="2" customWidth="1"/>
     <col min="6" max="6" width="32.88671875" customWidth="1"/>
     <col min="7" max="7" width="24.77734375" customWidth="1"/>
+    <col min="8" max="8" width="36.77734375" customWidth="1"/>
+    <col min="9" max="9" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="46.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="46.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>38</v>
       </c>
@@ -776,7 +802,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
@@ -787,7 +813,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -809,8 +835,14 @@
       <c r="G4" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="H4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -827,7 +859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>51</v>
       </c>
@@ -844,7 +876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -861,7 +893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -872,7 +904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -895,7 +927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -906,7 +938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -917,7 +949,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -928,7 +960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -950,8 +982,14 @@
       <c r="G13" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="H13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -970,7 +1008,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -981,7 +1019,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -1021,6 +1059,7 @@
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A19:G19"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>